<commit_message>
add filter for wrong inputs
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -7,9 +7,9 @@
     <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Hans_otg" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Hins_otg" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Klaus_otg" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Meier_otg" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Mueller_otg" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Schulze_otg" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -28,7 +28,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill/>
     </fill>
@@ -37,17 +37,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="0000FF00"/>
+        <fgColor rgb="00FFFF00"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00FF0000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00FFFF00"/>
+        <fgColor rgb="0000FF00"/>
       </patternFill>
     </fill>
   </fills>
@@ -63,11 +58,10 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="0" fillId="2" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="0" fillId="3" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="4" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -377,48 +371,48 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" t="inlineStr">
         <is>
           <t>Berlin</t>
         </is>
       </c>
-      <c r="C1" s="2" t="inlineStr">
+      <c r="C1" t="inlineStr">
         <is>
           <t>Hamburg</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="3" t="inlineStr">
+      <c r="A2" s="1" t="inlineStr">
         <is>
           <t>Nachname</t>
         </is>
       </c>
-      <c r="B2" s="1" t="inlineStr">
-        <is>
-          <t>am Deich</t>
-        </is>
-      </c>
-      <c r="C2" s="2" t="inlineStr">
-        <is>
-          <t>Postweg</t>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Burgallee</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Feldplatz</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Mueller</t>
-        </is>
-      </c>
-      <c r="B4" s="1" t="inlineStr">
-        <is>
-          <t>10</t>
+          <t>Meier</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>4</t>
         </is>
       </c>
       <c r="C4" s="2" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>6</t>
         </is>
       </c>
     </row>
@@ -433,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -442,31 +436,46 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>Berlin</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
         <is>
           <t>Hamburg</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="3" t="inlineStr">
+      <c r="A2" s="1" t="inlineStr">
         <is>
           <t>Nachname</t>
         </is>
       </c>
-      <c r="B2" s="1" t="inlineStr">
+      <c r="B2" s="2" t="inlineStr">
+        <is>
+          <t>am Deich</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
         <is>
           <t>Postweg</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="inlineStr">
+      <c r="A4" t="inlineStr">
         <is>
           <t>Mueller</t>
         </is>
       </c>
-      <c r="B4" s="1" t="inlineStr">
+      <c r="B4" s="2" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
         <is>
           <t>8</t>
         </is>
@@ -483,7 +492,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -492,19 +501,14 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="B1" s="4" t="inlineStr">
+      <c r="B1" s="3" t="inlineStr">
         <is>
           <t>Berlin</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>Hamburg</t>
-        </is>
-      </c>
     </row>
     <row r="2">
-      <c r="A2" s="3" t="inlineStr">
+      <c r="A2" s="1" t="inlineStr">
         <is>
           <t>Nachname</t>
         </is>
@@ -514,46 +518,24 @@
           <t>Burgallee</t>
         </is>
       </c>
-      <c r="C2" s="1" t="inlineStr">
+      <c r="C2" s="2" t="inlineStr">
         <is>
           <t>am Deich</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Feldplatz</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Meier</t>
+          <t>Schulze</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="D4" s="1" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Schulze</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
           <t>3</t>
         </is>
       </c>
-      <c r="C5" s="1" t="inlineStr">
+      <c r="C4" s="2" t="inlineStr">
         <is>
           <t>9</t>
         </is>

</xml_diff>